<commit_message>
Cruise passes for new PatternUtils strategy
</commit_message>
<xml_diff>
--- a/test/data/spreadsheets/ART-687-10-CODYesPeriod1_TwoUpdates.xlsx
+++ b/test/data/spreadsheets/ART-687-10-CODYesPeriod1_TwoUpdates.xlsx
@@ -1980,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1991,7 +1991,7 @@
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1999,47 +1999,48 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="14">
+        <v>40544</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="14">
         <v>40724</v>
-      </c>
-      <c r="B2" s="13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="14">
-        <v>40908</v>
       </c>
       <c r="B3" s="13">
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="42">
+    <row r="4" spans="1:3">
+      <c r="A4" s="14">
+        <v>40908</v>
+      </c>
+      <c r="B4" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="42">
         <v>41181</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B5" s="43">
         <v>2804.347826086957</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="42">
-        <v>41546</v>
-      </c>
-      <c r="B5" s="43">
-        <v>5842.3913043478269</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" s="42">
         <v>41546</v>
       </c>
       <c r="B6" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>5842.3913043478269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="42">
         <v>42033</v>
       </c>
@@ -2047,7 +2048,7 @@
         <v>7010.869565217391</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" s="42">
         <v>42398</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>4673.913043478261</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9" s="42">
         <v>42764</v>
       </c>

</xml_diff>